<commit_message>
Reduced decoupling caps on VREG to address issue #3
</commit_message>
<xml_diff>
--- a/wisp5-bom.xlsx
+++ b/wisp5-bom.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9885"/>
   </bookViews>
   <sheets>
-    <sheet name="wisp-5-0" sheetId="1" r:id="rId1"/>
+    <sheet name="wisp5-bom" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="196">
   <si>
     <t>Designator</t>
   </si>
@@ -89,7 +89,7 @@
     <t>C3, C8</t>
   </si>
   <si>
-    <t>1uF</t>
+    <t>0.1uF</t>
   </si>
   <si>
     <t>0402</t>
@@ -98,10 +98,10 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>GRM155R61A105KE15D</t>
-  </si>
-  <si>
-    <t>490-3890-1-ND</t>
+    <t>GRM155R71C104KA88D</t>
+  </si>
+  <si>
+    <t>490-3261-1-ND</t>
   </si>
   <si>
     <t>C4</t>
@@ -612,19 +612,13 @@
   </si>
   <si>
     <t>Header, 2-Pin</t>
-  </si>
-  <si>
-    <t>DNP=Do Not Populate</t>
-  </si>
-  <si>
-    <t>WISP 5.1 Bill Of Materials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -637,19 +631,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -699,19 +680,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,74 +1002,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="3" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -1102,33 +1104,33 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -1143,27 +1145,27 @@
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K4" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -1178,27 +1180,27 @@
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
@@ -1213,29 +1215,27 @@
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K6" s="3">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
@@ -1250,27 +1250,27 @@
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
@@ -1285,27 +1285,27 @@
         <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
@@ -1323,53 +1323,53 @@
         <v>28</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="K10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1378,33 +1378,33 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="K11" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -1413,103 +1413,103 @@
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>64</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
@@ -1518,60 +1518,60 @@
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="K15" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="K16" s="3">
         <v>1</v>
@@ -1579,13 +1579,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>98</v>
@@ -1603,10 +1603,10 @@
         <v>100</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K17" s="3">
         <v>1</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>98</v>
@@ -1638,10 +1638,10 @@
         <v>100</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="K18" s="3">
         <v>1</v>
@@ -1649,13 +1649,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>98</v>
@@ -1673,24 +1673,24 @@
         <v>100</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>98</v>
@@ -1708,10 +1708,10 @@
         <v>100</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K20" s="3">
         <v>2</v>
@@ -1719,13 +1719,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>98</v>
@@ -1743,80 +1743,80 @@
         <v>100</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="K21" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="K22" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="K23" s="3">
         <v>1</v>
@@ -1824,34 +1824,34 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="K24" s="3">
         <v>1</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
@@ -1868,25 +1868,25 @@
         <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="K25" s="3">
         <v>1</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
@@ -1903,25 +1903,25 @@
         <v>12</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="K26" s="3">
         <v>1</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>12</v>
@@ -1938,25 +1938,25 @@
         <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="K27" s="3">
         <v>1</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>12</v>
@@ -1973,25 +1973,25 @@
         <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="K28" s="3">
         <v>1</v>
@@ -1999,34 +1999,34 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>12</v>
+        <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="K29" s="3">
         <v>1</v>
@@ -2034,34 +2034,34 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>12</v>
+        <v>182</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>175</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>177</v>
+        <v>16</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>178</v>
+        <v>14</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>179</v>
+        <v>12</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
       <c r="K30" s="3">
         <v>1</v>
@@ -2069,9 +2069,9 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B31" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2084,7 +2084,7 @@
         <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>14</v>
@@ -2104,25 +2104,25 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>12</v>
@@ -2139,25 +2139,25 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B33" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>12</v>
@@ -2174,25 +2174,25 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B34" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>12</v>
@@ -2209,25 +2209,25 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>12</v>
@@ -2242,57 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K36" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
   </sheetData>
-  <sortState ref="A3:M36">
-    <sortCondition ref="B3:B36"/>
-    <sortCondition ref="A3:A36"/>
-    <sortCondition ref="C3:C36"/>
-  </sortState>
-  <mergeCells count="1">
-    <mergeCell ref="B38:D38"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>